<commit_message>
Task[13] v1 Info boxes and value boxes for each emotions.
   - Add correct icons for each emotions.
   - Add weights for each emotions. These will be used for weighing the heaviest emotion.
</commit_message>
<xml_diff>
--- a/R/emotions-final.xlsx
+++ b/R/emotions-final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\CIT-U\Masters of Computer Science\Capstone - Thesis\Emotions Detection and Analysis\EmoTector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\CIT-U\Masters of Computer Science\Capstone - Thesis\Emotions Detection and Analysis\EmoTector\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Anger" sheetId="5" r:id="rId5"/>
     <sheet name="+ Words" sheetId="6" r:id="rId6"/>
     <sheet name="- Words" sheetId="7" r:id="rId7"/>
+    <sheet name="Constrasting Conjunctions" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6900" uniqueCount="6850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6923" uniqueCount="6872">
   <si>
     <t>lowest</t>
   </si>
@@ -20580,13 +20581,79 @@
   </si>
   <si>
     <t>somehow</t>
+  </si>
+  <si>
+    <t>but</t>
+  </si>
+  <si>
+    <t>although</t>
+  </si>
+  <si>
+    <t>though</t>
+  </si>
+  <si>
+    <t>whereas</t>
+  </si>
+  <si>
+    <t>yet</t>
+  </si>
+  <si>
+    <t>nevertheless</t>
+  </si>
+  <si>
+    <t>however</t>
+  </si>
+  <si>
+    <t>still</t>
+  </si>
+  <si>
+    <t>notwithstanding</t>
+  </si>
+  <si>
+    <t>despite</t>
+  </si>
+  <si>
+    <t>regardless</t>
+  </si>
+  <si>
+    <t>Conjunctions</t>
+  </si>
+  <si>
+    <t>nonetheless</t>
+  </si>
+  <si>
+    <t>even so</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>neither</t>
+  </si>
+  <si>
+    <t>nowhere</t>
+  </si>
+  <si>
+    <t>nobody</t>
+  </si>
+  <si>
+    <t>hardly</t>
+  </si>
+  <si>
+    <t>scarely</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -20630,6 +20697,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -20657,7 +20731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -20675,6 +20749,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20996,7 +21071,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21513,6 +21588,9 @@
       <c r="A26" s="10" t="s">
         <v>6846</v>
       </c>
+      <c r="B26" s="8" t="s">
+        <v>6870</v>
+      </c>
       <c r="C26" s="5" t="s">
         <v>202</v>
       </c>
@@ -21527,6 +21605,12 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>6864</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>6871</v>
+      </c>
       <c r="C27" s="5" t="s">
         <v>203</v>
       </c>
@@ -21541,6 +21625,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>6865</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>205</v>
       </c>
@@ -21555,6 +21642,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>6869</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>206</v>
       </c>
@@ -21569,6 +21659,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>6866</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>207</v>
       </c>
@@ -21583,6 +21676,9 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>6867</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>127</v>
       </c>
@@ -21597,6 +21693,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>6868</v>
+      </c>
       <c r="C32" s="5" t="s">
         <v>223</v>
       </c>
@@ -57869,4 +57968,99 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6861</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>6850</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>6856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>6862</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>6854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>6863</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>6855</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>6857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>6858</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>6851</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>6852</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>6853</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>6859</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>5964</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>6860</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Task[13] Box for each emotions and added refine bag-of-words.
   - Update final-list-of-emotions.xlsx.
   - Apply conditions on the boxes.
</commit_message>
<xml_diff>
--- a/R/emotions-final.xlsx
+++ b/R/emotions-final.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Anger" sheetId="5" r:id="rId5"/>
     <sheet name="+ Words" sheetId="6" r:id="rId6"/>
     <sheet name="- Words" sheetId="7" r:id="rId7"/>
-    <sheet name="Constrasting Conjunctions" sheetId="8" r:id="rId8"/>
+    <sheet name="Constrasting Conjunctions" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6923" uniqueCount="6872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6936" uniqueCount="6878">
   <si>
     <t>lowest</t>
   </si>
@@ -20647,13 +20647,31 @@
   </si>
   <si>
     <t>scarely</t>
+  </si>
+  <si>
+    <t>literally</t>
+  </si>
+  <si>
+    <t>mostly</t>
+  </si>
+  <si>
+    <t>quite</t>
+  </si>
+  <si>
+    <t>rather</t>
+  </si>
+  <si>
+    <t>faintly</t>
+  </si>
+  <si>
+    <t>vaguely</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -20704,6 +20722,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -20728,10 +20753,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -20749,10 +20775,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -21071,7 +21100,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21628,6 +21657,9 @@
       <c r="A28" s="8" t="s">
         <v>6865</v>
       </c>
+      <c r="B28" s="8" t="s">
+        <v>6874</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>205</v>
       </c>
@@ -21645,6 +21677,9 @@
       <c r="A29" s="8" t="s">
         <v>6869</v>
       </c>
+      <c r="B29" s="8" t="s">
+        <v>6875</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>206</v>
       </c>
@@ -21662,6 +21697,9 @@
       <c r="A30" s="8" t="s">
         <v>6866</v>
       </c>
+      <c r="B30" s="8" t="s">
+        <v>6876</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>207</v>
       </c>
@@ -21679,6 +21717,9 @@
       <c r="A31" s="8" t="s">
         <v>6867</v>
       </c>
+      <c r="B31" s="8" t="s">
+        <v>6877</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>127</v>
       </c>
@@ -21845,7 +21886,9 @@
       <c r="E42" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="F42" s="5"/>
+      <c r="F42" s="5" t="s">
+        <v>3516</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
@@ -21857,6 +21900,9 @@
       <c r="E43" s="5" t="s">
         <v>404</v>
       </c>
+      <c r="F43" s="5" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
@@ -21868,6 +21914,9 @@
       <c r="E44" s="5" t="s">
         <v>417</v>
       </c>
+      <c r="F44" s="5" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
@@ -21879,6 +21928,9 @@
       <c r="E45" s="5" t="s">
         <v>418</v>
       </c>
+      <c r="F45" s="5" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C46" s="5" t="s">
@@ -21889,6 +21941,9 @@
       </c>
       <c r="E46" s="5" t="s">
         <v>419</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>6872</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -21902,6 +21957,9 @@
       <c r="E47" s="5" t="s">
         <v>433</v>
       </c>
+      <c r="F47" s="5" t="s">
+        <v>6873</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C48" s="5" t="s">
@@ -21913,8 +21971,11 @@
       <c r="E48" s="5" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="5" t="s">
+        <v>5140</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="5" t="s">
         <v>267</v>
       </c>
@@ -21924,8 +21985,11 @@
       <c r="E49" s="5" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="5" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="5" t="s">
         <v>269</v>
       </c>
@@ -21935,8 +21999,11 @@
       <c r="E50" s="5" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C51" s="5" t="s">
         <v>270</v>
       </c>
@@ -21947,7 +22014,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C52" s="5" t="s">
         <v>272</v>
       </c>
@@ -21958,7 +22025,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C53" s="5" t="s">
         <v>275</v>
       </c>
@@ -21969,7 +22036,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C54" s="5" t="s">
         <v>276</v>
       </c>
@@ -21980,7 +22047,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C55" s="5" t="s">
         <v>279</v>
       </c>
@@ -21991,7 +22058,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C56" s="5" t="s">
         <v>280</v>
       </c>
@@ -22002,7 +22069,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C57" s="5" t="s">
         <v>281</v>
       </c>
@@ -22013,7 +22080,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C58" s="5" t="s">
         <v>286</v>
       </c>
@@ -22024,7 +22091,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C59" s="5" t="s">
         <v>287</v>
       </c>
@@ -22035,7 +22102,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C60" s="5" t="s">
         <v>298</v>
       </c>
@@ -22046,7 +22113,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C61" s="5" t="s">
         <v>301</v>
       </c>
@@ -22057,7 +22124,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C62" s="5" t="s">
         <v>303</v>
       </c>
@@ -22068,7 +22135,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C63" s="5" t="s">
         <v>304</v>
       </c>
@@ -22079,7 +22146,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C64" s="5" t="s">
         <v>308</v>
       </c>
@@ -57962,7 +58029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -57979,83 +58048,86 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="12"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>6861</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>6850</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>6856</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>6862</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="13" t="s">
         <v>6854</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>6863</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>6855</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>6857</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>6858</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>6851</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="13" t="s">
         <v>6852</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>6853</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="13" t="s">
         <v>6859</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>5964</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="13" t="s">
         <v>6860</v>
       </c>
     </row>

</xml_diff>